<commit_message>
updated documents and commented code
</commit_message>
<xml_diff>
--- a/Document/Requirement Traceability Matrix.xlsx
+++ b/Document/Requirement Traceability Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -302,6 +302,27 @@
   </si>
   <si>
     <t>Perform Functionlity Testing and prepare Unit Testnig doc to evaluate model</t>
+  </si>
+  <si>
+    <t>Chan PATIL</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Sahiti/Vinya</t>
+  </si>
+  <si>
+    <t>Chan/Aditya</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>Aditya/Ravi</t>
   </si>
 </sst>
 </file>
@@ -532,13 +553,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -823,7 +844,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E24" sqref="A24:XFD24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -863,18 +886,22 @@
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -888,8 +915,12 @@
       <c r="E3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -905,8 +936,12 @@
       <c r="E4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -918,14 +953,18 @@
       <c r="E5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -937,14 +976,18 @@
       <c r="E6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="22"/>
       <c r="D7" s="8" t="s">
         <v>29</v>
@@ -952,14 +995,18 @@
       <c r="E7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="22"/>
       <c r="D8" s="8" t="s">
         <v>32</v>
@@ -967,14 +1014,18 @@
       <c r="E8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="22"/>
       <c r="D9" s="8" t="s">
         <v>33</v>
@@ -982,14 +1033,18 @@
       <c r="E9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -1001,217 +1056,281 @@
       <c r="E10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="21" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
+      <c r="F17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
+      <c r="F19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
+      <c r="F21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
+      <c r="F23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
+      <c r="F25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="22" t="s">
         <v>48</v>
       </c>
@@ -1228,7 +1347,7 @@
       <c r="A27" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="15" t="s">
@@ -1241,7 +1360,7 @@
       <c r="A28" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="15" t="s">
@@ -1254,7 +1373,7 @@
       <c r="A29" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="15" t="s">
@@ -1267,7 +1386,7 @@
       <c r="A30" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="15" t="s">
@@ -1374,6 +1493,14 @@
   </sheetData>
   <autoFilter ref="A1:G35"/>
   <mergeCells count="18">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B10:B30"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C10:C15"/>
     <mergeCell ref="D16:D20"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
@@ -1384,14 +1511,6 @@
     <mergeCell ref="D21:D25"/>
     <mergeCell ref="D26:D30"/>
     <mergeCell ref="D10:D15"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B10:B30"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C10:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>